<commit_message>
Zener was deleted prooerties was changed to 12V 20A
</commit_message>
<xml_diff>
--- a/H0FR70/Released/BOM/H0FR70.xlsx
+++ b/H0FR70/Released/BOM/H0FR70.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="H0FR70" localSheetId="0">Sheet1!$A$1:$H$23</definedName>
+    <definedName name="H0FR70" localSheetId="0">Sheet1!$A$1:$H$22</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="104">
   <si>
     <t>Qty</t>
   </si>
@@ -238,18 +238,6 @@
     <t>https://octopart.com/bss123-on+semiconductor-20837328?r=sp</t>
   </si>
   <si>
-    <t>BZT52C2V0S-7-F</t>
-  </si>
-  <si>
-    <t>D4</t>
-  </si>
-  <si>
-    <t>Diodes Inc.</t>
-  </si>
-  <si>
-    <t>https://octopart.com/bzt52c2v0s-7-f-diodes+inc.-7151792?r=sp</t>
-  </si>
-  <si>
     <t>FB-TDK_MMZ1608Y300B</t>
   </si>
   <si>
@@ -362,9 +350,6 @@
   </si>
   <si>
     <t>CAP CER  10% X7R 0603</t>
-  </si>
-  <si>
-    <t>Zener diode 2V 10A 200W</t>
   </si>
   <si>
     <t>MCU 32-bit ARM Cortex M0 RISC 128KB Flash 2.5V/3.3V 48-Pin UFQFPN EP Frame</t>
@@ -704,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,13 +712,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -756,7 +741,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>30</v>
@@ -779,7 +764,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
@@ -799,10 +784,10 @@
         <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
@@ -825,7 +810,7 @@
         <v>48</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>49</v>
@@ -842,22 +827,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -865,22 +850,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="F7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -888,10 +873,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D8" s="1">
         <v>304020019</v>
@@ -900,10 +885,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -917,16 +902,16 @@
         <v>62</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -934,22 +919,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -957,22 +942,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>88</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -980,22 +965,22 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>90</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>91</v>
+        <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>92</v>
+        <v>18</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>90</v>
+        <v>43</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>93</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1003,10 +988,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>18</v>
@@ -1015,21 +1000,21 @@
         <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>18</v>
@@ -1038,21 +1023,21 @@
         <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>18</v>
@@ -1061,21 +1046,21 @@
         <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>18</v>
@@ -1084,10 +1069,10 @@
         <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1095,22 +1080,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1118,22 +1103,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1141,22 +1126,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1164,22 +1149,22 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>9</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1187,68 +1172,45 @@
         <v>1</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>94</v>
+      <c r="B22" s="1">
+        <v>34.402999999999999</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>95</v>
+        <v>5</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
+      </c>
+      <c r="F22" s="1">
+        <v>34.402999999999999</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>1</v>
-      </c>
-      <c r="B23" s="1">
-        <v>34.402999999999999</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="1">
-        <v>34.402999999999999</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PDF fixed R8 changed (2k2 -> 1k) BOM modified
</commit_message>
<xml_diff>
--- a/H0FR70/Released/BOM/H0FR70.xlsx
+++ b/H0FR70/Released/BOM/H0FR70.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="H0FR70" localSheetId="0">Sheet1!$A$1:$H$22</definedName>
+    <definedName name="H0FR70" localSheetId="0">Sheet1!$A$1:$H$21</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="103">
   <si>
     <t>Qty</t>
   </si>
@@ -169,9 +169,6 @@
     <t>1k</t>
   </si>
   <si>
-    <t>R10</t>
-  </si>
-  <si>
     <t>RC0603JR-071KL</t>
   </si>
   <si>
@@ -190,12 +187,6 @@
     <t>https://octopart.com/search?q=RC0603FR-07270RL&amp;start=0</t>
   </si>
   <si>
-    <t>2k2</t>
-  </si>
-  <si>
-    <t>R8</t>
-  </si>
-  <si>
     <t>4.7uF</t>
   </si>
   <si>
@@ -365,16 +356,30 @@
   </si>
   <si>
     <t>https://octopart.com/34.403-altech-859840?r=sp#</t>
+  </si>
+  <si>
+    <t>Orange 0603 130° Clear 54 mcd 2 V Surface Mount ChipLED ;</t>
+  </si>
+  <si>
+    <t>R8,R10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,16 +402,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -689,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,13 +722,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
@@ -741,7 +751,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>30</v>
@@ -764,7 +774,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
@@ -784,10 +794,10 @@
         <v>29</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>30</v>
@@ -804,22 +814,22 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -827,22 +837,22 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>81</v>
+        <v>70</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -850,22 +860,22 @@
         <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -873,10 +883,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D8" s="1">
         <v>304020019</v>
@@ -885,10 +895,10 @@
         <v>8</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -896,22 +906,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -919,22 +929,22 @@
         <v>1</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="F10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -942,22 +952,22 @@
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -965,10 +975,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>18</v>
@@ -977,21 +987,21 @@
         <v>13</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>18</v>
@@ -1000,21 +1010,21 @@
         <v>13</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>18</v>
@@ -1023,21 +1033,21 @@
         <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>18</v>
@@ -1046,10 +1056,10 @@
         <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1057,22 +1067,22 @@
         <v>1</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>54</v>
+        <v>14</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1080,22 +1090,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>15</v>
+        <v>38</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1103,22 +1113,22 @@
         <v>1</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1126,22 +1136,22 @@
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>8</v>
+        <v>67</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>9</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1149,75 +1159,57 @@
         <v>1</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>68</v>
+        <v>88</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>1</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>90</v>
+      <c r="B21" s="1">
+        <v>34.402999999999999</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
+      </c>
+      <c r="F21" s="1">
+        <v>34.402999999999999</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1">
-        <v>34.402999999999999</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="1">
-        <v>34.402999999999999</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G27">
-    <sortCondition ref="C1"/>
+  <sortState ref="A2:G22">
+    <sortCondition ref="C4"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="G7" r:id="rId1"/>
+    <hyperlink ref="G6" r:id="rId2"/>
+    <hyperlink ref="G17" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>